<commit_message>
update combinations for other entries
</commit_message>
<xml_diff>
--- a/data/object25_info.xlsx
+++ b/data/object25_info.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NIkan\Desktop\Deep Halftoning\Github\Deep-Halftoning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{96FEEEB7-0B64-4A4F-BB51-93CA555F9EBB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321FD5DC-2EE7-4325-89CE-7D8DE956E6C5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="object150_info" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t>Idx</t>
   </si>
@@ -570,11 +570,14 @@
   <si>
     <t>NOTE: INDEXES are based on EXCEL not IDX column - EVERY THING -1</t>
   </si>
+  <si>
+    <t>82+85+92+104+118+129</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1149,16 +1152,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>229382</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>66932</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>524657</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>181232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1181,7 +1184,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7915275" y="133350"/>
+          <a:off x="6381750" y="57150"/>
           <a:ext cx="5601482" cy="1838582"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1490,11 +1493,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="F91" sqref="F91"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1870,6 +1873,9 @@
       <c r="E16" s="2">
         <v>796</v>
       </c>
+      <c r="F16" s="2">
+        <v>60</v>
+      </c>
       <c r="G16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1963,6 +1969,9 @@
       <c r="E20" s="2">
         <v>217</v>
       </c>
+      <c r="F20" s="2">
+        <v>103</v>
+      </c>
       <c r="G20" s="2" t="s">
         <v>22</v>
       </c>
@@ -2008,6 +2017,9 @@
       <c r="E22" s="2">
         <v>306</v>
       </c>
+      <c r="F22" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="G22" s="2" t="s">
         <v>153</v>
       </c>
@@ -2857,6 +2869,9 @@
       <c r="E60" s="1">
         <v>18</v>
       </c>
+      <c r="F60" s="1">
+        <v>16</v>
+      </c>
       <c r="G60" s="1" t="s">
         <v>60</v>
       </c>
@@ -3343,6 +3358,9 @@
       <c r="E82" s="1">
         <v>25</v>
       </c>
+      <c r="F82" s="1">
+        <v>22</v>
+      </c>
       <c r="G82" s="1" t="s">
         <v>81</v>
       </c>
@@ -3406,6 +3424,9 @@
       <c r="E85" s="1">
         <v>39</v>
       </c>
+      <c r="F85" s="1">
+        <v>22</v>
+      </c>
       <c r="G85" s="1" t="s">
         <v>84</v>
       </c>
@@ -3556,6 +3577,9 @@
       <c r="E92" s="1">
         <v>12</v>
       </c>
+      <c r="F92" s="1">
+        <v>22</v>
+      </c>
       <c r="G92" s="1" t="s">
         <v>91</v>
       </c>
@@ -3769,6 +3793,9 @@
       <c r="E102" s="1">
         <v>35</v>
       </c>
+      <c r="F102" s="1">
+        <v>45</v>
+      </c>
       <c r="G102" s="1" t="s">
         <v>101</v>
       </c>
@@ -3790,6 +3817,9 @@
       <c r="E103" s="1">
         <v>9</v>
       </c>
+      <c r="F103" s="1">
+        <v>20</v>
+      </c>
       <c r="G103" s="1" t="s">
         <v>102</v>
       </c>
@@ -3811,6 +3841,9 @@
       <c r="E104" s="1">
         <v>55</v>
       </c>
+      <c r="F104" s="1">
+        <v>22</v>
+      </c>
       <c r="G104" s="1" t="s">
         <v>103</v>
       </c>
@@ -4111,6 +4144,9 @@
       <c r="E118" s="1">
         <v>30</v>
       </c>
+      <c r="F118" s="1">
+        <v>22</v>
+      </c>
       <c r="G118" s="1" t="s">
         <v>117</v>
       </c>
@@ -4258,6 +4294,9 @@
       <c r="E125" s="1">
         <v>83</v>
       </c>
+      <c r="F125" s="1">
+        <v>45</v>
+      </c>
       <c r="G125" s="1" t="s">
         <v>124</v>
       </c>
@@ -4342,6 +4381,9 @@
       <c r="E129" s="1">
         <v>36</v>
       </c>
+      <c r="F129" s="1">
+        <v>22</v>
+      </c>
       <c r="G129" s="1" t="s">
         <v>128</v>
       </c>
@@ -4663,6 +4705,9 @@
       <c r="E144" s="1">
         <v>59</v>
       </c>
+      <c r="F144" s="1">
+        <v>45</v>
+      </c>
       <c r="G144" s="1" t="s">
         <v>143</v>
       </c>
@@ -4704,6 +4749,9 @@
       </c>
       <c r="E146" s="1">
         <v>19</v>
+      </c>
+      <c r="F146" s="1">
+        <v>45</v>
       </c>
       <c r="G146" s="1" t="s">
         <v>145</v>

</xml_diff>

<commit_message>
use dictionary to represent replacements
</commit_message>
<xml_diff>
--- a/data/object25_info.xlsx
+++ b/data/object25_info.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NIkan\Desktop\Deep Halftoning\Github\Deep-Halftoning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E2E164-3C66-4127-AC96-0CE379554CBB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09532E6-F0B9-4759-9DFA-0D5CE353865D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="object150_info" sheetId="1" r:id="rId1"/>
+    <sheet name="Final" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="185">
   <si>
     <t>Idx</t>
   </si>
@@ -584,6 +585,45 @@
   </si>
   <si>
     <t>80+91+143+145</t>
+  </si>
+  <si>
+    <t>26+49+85</t>
+  </si>
+  <si>
+    <t>11+52+54</t>
+  </si>
+  <si>
+    <t>45+36</t>
+  </si>
+  <si>
+    <t>30+47</t>
+  </si>
+  <si>
+    <t>20+31+34+46+57+65+70+71+76+100+111</t>
+  </si>
+  <si>
+    <t>35+69</t>
+  </si>
+  <si>
+    <t>9+67</t>
+  </si>
+  <si>
+    <t>81+84+91+103+117+128</t>
+  </si>
+  <si>
+    <t>141+129+110+61+22</t>
+  </si>
+  <si>
+    <t>83+88</t>
+  </si>
+  <si>
+    <t>101+124+143+145</t>
+  </si>
+  <si>
+    <t>60+97+122</t>
+  </si>
+  <si>
+    <t>79+90+142+144</t>
   </si>
 </sst>
 </file>
@@ -1517,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="A76" activeCellId="22" sqref="A4:XFD4 A5:XFD5 A6:XFD6 A7:XFD7 A8:XFD8 A9:XFD9 A12:XFD12 A14:XFD14 A15:XFD15 A16:XFD16 A17:XFD17 A18:XFD18 A19:XFD19 A20:XFD20 A22:XFD22 A28:XFD28 A25:XFD25 A26:XFD26 A38:XFD38 A45:XFD45 A55:XFD55 A67:XFD67 A76:XFD76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4933,4 +4973,453 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13052BAF-6C36-4493-BFD1-A060262243E3}">
+  <dimension ref="A1:AA25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <f>C1*100</f>
+        <v>15.76</v>
+      </c>
+      <c r="C1" s="2">
+        <v>0.15759999999999999</v>
+      </c>
+      <c r="D1" s="2">
+        <v>43</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+    </row>
+    <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <f>C2*100</f>
+        <v>10.72</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.1072</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>8.7800000000000011</v>
+      </c>
+      <c r="C3" s="3">
+        <v>8.7800000000000003E-2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6.21</v>
+      </c>
+      <c r="C4" s="3">
+        <v>6.2100000000000002E-2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>73</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3.9800000000000004</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3.9800000000000002E-2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2.31</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2.3099999999999999E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>58</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.81</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.51</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.18</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.18E-2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>59</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.09E-2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.04E-2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.04E-2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>102</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="C17" s="2">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="C18" s="3">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="C19" s="3">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>27</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="C20" s="2">
+        <v>5.3E-3</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>37</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>44</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>54</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.16999999999999998</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>66</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="D24" s="2">
+        <v>38</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>75</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update DetailsNet training procedure
</commit_message>
<xml_diff>
--- a/data/object25_info.xlsx
+++ b/data/object25_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NIkan\Desktop\Deep Halftoning\Github\Deep-Halftoning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09532E6-F0B9-4759-9DFA-0D5CE353865D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC43088-257C-409F-AD16-9A04B9BEA2BE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="object150_info" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="184">
   <si>
     <t>Idx</t>
   </si>
@@ -567,9 +567,6 @@
   </si>
   <si>
     <t>142+130+111+62+23</t>
-  </si>
-  <si>
-    <t>NOTE: INDEXES are based on EXCEL not IDX column - EVERY THING -1</t>
   </si>
   <si>
     <t>82+85+92+104+118+129</t>
@@ -1557,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R151"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A76" activeCellId="22" sqref="A4:XFD4 A5:XFD5 A6:XFD6 A7:XFD7 A8:XFD8 A9:XFD9 A12:XFD12 A14:XFD14 A15:XFD15 A16:XFD16 A17:XFD17 A18:XFD18 A19:XFD19 A20:XFD20 A22:XFD22 A28:XFD28 A25:XFD25 A26:XFD26 A38:XFD38 A45:XFD45 A55:XFD55 A67:XFD67 A76:XFD76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="A1:G151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,9 +1860,7 @@
       <c r="G13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M13" s="4" t="s">
-        <v>166</v>
-      </c>
+      <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
@@ -2079,7 +2074,7 @@
         <v>306</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>153</v>
@@ -2442,7 +2437,7 @@
         <v>302</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>38</v>
@@ -2598,7 +2593,7 @@
         <v>298</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>45</v>
@@ -2826,7 +2821,7 @@
         <v>102</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>55</v>
@@ -3309,7 +3304,7 @@
         <v>29</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>154</v>
@@ -4979,8 +4974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13052BAF-6C36-4493-BFD1-A060262243E3}">
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5040,7 +5035,7 @@
         <v>0.1072</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
@@ -5116,7 +5111,7 @@
         <v>3.9800000000000002E-2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
@@ -5150,7 +5145,7 @@
         <v>1.8100000000000002E-2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>15</v>
@@ -5181,7 +5176,7 @@
         <v>1.5100000000000001E-2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>18</v>
@@ -5215,7 +5210,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>20</v>
@@ -5232,7 +5227,7 @@
         <v>1.09E-2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>21</v>
@@ -5249,7 +5244,7 @@
         <v>1.04E-2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>151</v>
@@ -5283,7 +5278,7 @@
         <v>9.7999999999999997E-3</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>153</v>
@@ -5328,7 +5323,7 @@
         <v>5.3E-3</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>152</v>
@@ -5345,7 +5340,7 @@
         <v>2.5999999999999999E-3</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>38</v>
@@ -5362,7 +5357,7 @@
         <v>2E-3</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>45</v>
@@ -5379,7 +5374,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>55</v>
@@ -5413,7 +5408,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>154</v>

</xml_diff>